<commit_message>
modif tableau audit seo
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mouatakide1\Desktop\p4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mouatakide1\Desktop\p4\p4\La-chouette-agence-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5781D5A-1148-41B2-AD1B-90361A2EF0B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68666421-6BCD-4063-806A-AC1E3C6F60CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="390" windowWidth="19050" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="0" windowWidth="19050" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Catégorie</t>
   </si>
@@ -46,13 +46,67 @@
   </si>
   <si>
     <t>(SEO ou accessiblité ?)</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>Pas de meta description</t>
+  </si>
+  <si>
+    <t>Content vide</t>
+  </si>
+  <si>
+    <t>Mettre une description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">police trop petite </t>
+  </si>
+  <si>
+    <t>- de 12px sur 60% du site</t>
+  </si>
+  <si>
+    <t>augmenter en rem ou en %</t>
+  </si>
+  <si>
+    <t>cibles tactiles trop petites</t>
+  </si>
+  <si>
+    <t>inférieur à 48px par 48 px</t>
+  </si>
+  <si>
+    <t xml:space="preserve">augmenter à 48 48px </t>
+  </si>
+  <si>
+    <t>accessibilité</t>
+  </si>
+  <si>
+    <t>couleurs d'arrière-plan et de premier plan n'ont pas un rapport de contraste suffisant</t>
+  </si>
+  <si>
+    <t>Le texte de 18 points ou 14 points en gras nécessite un rapport de contraste de 3: 1.</t>
+  </si>
+  <si>
+    <t>Tout autre texte a besoin d'un rapport de contraste de 4,5: 1.</t>
+  </si>
+  <si>
+    <t>pas un rapport de contraste suffisamment élevé</t>
+  </si>
+  <si>
+    <t>Les éléments d'en-tête ne sont pas dans un ordre séquentiel décroissant</t>
+  </si>
+  <si>
+    <t>Échec de l'audit des niveaux de titre du phare </t>
+  </si>
+  <si>
+    <t>utiliser les h1 h2 h3 etc,,,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,6 +132,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -113,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -121,6 +181,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,11 +400,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.77734375" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
@@ -397,36 +464,102 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
       <c r="E3" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
       <c r="E7" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="E8" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="E9" s="4" t="b">
         <v>0</v>
       </c>
@@ -1448,6 +1581,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modif pour un seo 100%
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mouatakide1\Desktop\p4\p4\La-chouette-agence-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68666421-6BCD-4063-806A-AC1E3C6F60CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4130280-B29C-4E1A-8D3E-A7067CB80EB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="0" windowWidth="19050" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Catégorie</t>
   </si>
@@ -66,18 +66,6 @@
     <t>- de 12px sur 60% du site</t>
   </si>
   <si>
-    <t>augmenter en rem ou en %</t>
-  </si>
-  <si>
-    <t>cibles tactiles trop petites</t>
-  </si>
-  <si>
-    <t>inférieur à 48px par 48 px</t>
-  </si>
-  <si>
-    <t xml:space="preserve">augmenter à 48 48px </t>
-  </si>
-  <si>
     <t>accessibilité</t>
   </si>
   <si>
@@ -100,6 +88,9 @@
   </si>
   <si>
     <t>utiliser les h1 h2 h3 etc,,,</t>
+  </si>
+  <si>
+    <t>augmenter a 12px</t>
   </si>
 </sst>
 </file>
@@ -400,17 +391,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="66.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="74.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
@@ -459,9 +450,7 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -476,9 +465,7 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -491,108 +478,75 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="b">
-        <v>0</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="4" t="b">
-        <v>0</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="4" t="b">
-        <v>0</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="4" t="b">
-        <v>0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="4" t="b">
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>